<commit_message>
updated with additional dataset
</commit_message>
<xml_diff>
--- a/results/segment_times_multi-class.xlsx
+++ b/results/segment_times_multi-class.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vigneshselvaraj/Library/CloudStorage/Box-Box/phd/projects/energy_monitoring/research_work/machine_fault_identification/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5FA901-7AEC-F141-AADA-BE212AE3905C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE36D1F-CB6D-9845-A173-8531936A6CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="-13740" windowWidth="38400" windowHeight="19760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="15" sheetId="4" r:id="rId1"/>
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66D6986-0F2E-4E10-9668-9883B9C6C450}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -505,40 +505,40 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>0.987626</v>
+        <v>0.97273100000000001</v>
       </c>
       <c r="C3" s="3">
-        <v>2.4849999999999998E-3</v>
+        <v>2.431E-3</v>
       </c>
       <c r="D3" s="3">
-        <v>0.98819800000000002</v>
+        <v>0.99520500000000001</v>
       </c>
       <c r="E3" s="3">
-        <v>2.2200000000000002E-3</v>
+        <v>1.003E-3</v>
       </c>
       <c r="F3">
-        <v>0.82858600000000004</v>
+        <v>0.95455699999999999</v>
       </c>
       <c r="G3">
-        <v>8.9479999999999994E-3</v>
+        <v>1.977E-3</v>
       </c>
       <c r="H3">
-        <v>0.993085</v>
+        <v>0.97436999999999996</v>
       </c>
       <c r="I3" s="4">
-        <v>1.9759999999999999E-3</v>
+        <v>2.496E-3</v>
       </c>
       <c r="J3">
-        <v>0.99573699999999998</v>
+        <v>0.99832500000000002</v>
       </c>
       <c r="K3">
-        <v>1.603E-3</v>
+        <v>4.0900000000000002E-4</v>
       </c>
       <c r="L3">
-        <v>0.99880400000000003</v>
+        <v>0.99948899999999996</v>
       </c>
       <c r="M3">
-        <v>8.1499999999999997E-4</v>
+        <v>1.54E-4</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -546,40 +546,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>0.99094499999999996</v>
+        <v>0.94438599999999995</v>
       </c>
       <c r="C4" s="3">
-        <v>1.7279999999999999E-3</v>
+        <v>4.2579999999999996E-3</v>
       </c>
       <c r="D4" s="3">
-        <v>0.99134199999999995</v>
+        <v>0.99041699999999999</v>
       </c>
       <c r="E4" s="3">
-        <v>1.707E-3</v>
+        <v>2.0240000000000002E-3</v>
       </c>
       <c r="F4">
-        <v>0.87307400000000002</v>
+        <v>0.90617400000000004</v>
       </c>
       <c r="G4">
-        <v>6.2760000000000003E-3</v>
+        <v>2.9260000000000002E-3</v>
       </c>
       <c r="H4">
-        <v>0.99510799999999999</v>
+        <v>0.94709500000000002</v>
       </c>
       <c r="I4" s="4">
-        <v>1.3649999999999999E-3</v>
+        <v>4.3420000000000004E-3</v>
       </c>
       <c r="J4">
-        <v>0.99665499999999996</v>
+        <v>0.996672</v>
       </c>
       <c r="K4">
-        <v>1.5299999999999999E-3</v>
+        <v>8.5599999999999999E-4</v>
       </c>
       <c r="L4">
-        <v>0.99916099999999997</v>
+        <v>0.998942</v>
       </c>
       <c r="M4">
-        <v>5.5800000000000001E-4</v>
+        <v>2.92E-4</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -587,40 +587,40 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>0.987626</v>
+        <v>0.97273100000000001</v>
       </c>
       <c r="C5" s="3">
-        <v>2.4849999999999998E-3</v>
+        <v>2.431E-3</v>
       </c>
       <c r="D5" s="3">
-        <v>0.98819800000000002</v>
+        <v>0.99520500000000001</v>
       </c>
       <c r="E5" s="3">
-        <v>2.2200000000000002E-3</v>
+        <v>1.003E-3</v>
       </c>
       <c r="F5">
-        <v>0.82858600000000004</v>
+        <v>0.95455699999999999</v>
       </c>
       <c r="G5">
-        <v>8.9479999999999994E-3</v>
+        <v>1.977E-3</v>
       </c>
       <c r="H5">
-        <v>0.993085</v>
+        <v>0.97436999999999996</v>
       </c>
       <c r="I5" s="4">
-        <v>1.9759999999999999E-3</v>
+        <v>2.496E-3</v>
       </c>
       <c r="J5">
-        <v>0.99573699999999998</v>
+        <v>0.99832500000000002</v>
       </c>
       <c r="K5">
-        <v>1.603E-3</v>
+        <v>4.0900000000000002E-4</v>
       </c>
       <c r="L5">
-        <v>0.99880400000000003</v>
+        <v>0.99948899999999996</v>
       </c>
       <c r="M5">
-        <v>8.1499999999999997E-4</v>
+        <v>1.54E-4</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -628,40 +628,40 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>0.987626</v>
+        <v>0.97273100000000001</v>
       </c>
       <c r="C6" s="3">
-        <v>2.4849999999999998E-3</v>
+        <v>2.431E-3</v>
       </c>
       <c r="D6" s="3">
-        <v>0.98819800000000002</v>
+        <v>0.99520500000000001</v>
       </c>
       <c r="E6" s="3">
-        <v>2.2200000000000002E-3</v>
+        <v>1.003E-3</v>
       </c>
       <c r="F6">
-        <v>0.82858600000000004</v>
+        <v>0.95455699999999999</v>
       </c>
       <c r="G6">
-        <v>8.9479999999999994E-3</v>
+        <v>1.977E-3</v>
       </c>
       <c r="H6">
-        <v>0.993085</v>
+        <v>0.97436999999999996</v>
       </c>
       <c r="I6" s="4">
-        <v>1.9759999999999999E-3</v>
+        <v>2.496E-3</v>
       </c>
       <c r="J6">
-        <v>0.99573699999999998</v>
+        <v>0.99832500000000002</v>
       </c>
       <c r="K6">
-        <v>1.603E-3</v>
+        <v>4.0900000000000002E-4</v>
       </c>
       <c r="L6">
-        <v>0.99880400000000003</v>
+        <v>0.99948899999999996</v>
       </c>
       <c r="M6">
-        <v>8.1499999999999997E-4</v>
+        <v>1.54E-4</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -669,40 +669,40 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>0.987626</v>
+        <v>0.97273100000000001</v>
       </c>
       <c r="C7" s="3">
-        <v>2.4849999999999998E-3</v>
+        <v>2.431E-3</v>
       </c>
       <c r="D7" s="3">
-        <v>0.98819800000000002</v>
+        <v>0.99520500000000001</v>
       </c>
       <c r="E7" s="3">
-        <v>2.2200000000000002E-3</v>
+        <v>1.003E-3</v>
       </c>
       <c r="F7">
-        <v>0.82858600000000004</v>
+        <v>0.95455699999999999</v>
       </c>
       <c r="G7">
-        <v>8.9479999999999994E-3</v>
+        <v>1.977E-3</v>
       </c>
       <c r="H7">
-        <v>0.993085</v>
+        <v>0.97436999999999996</v>
       </c>
       <c r="I7" s="4">
-        <v>1.9759999999999999E-3</v>
+        <v>2.496E-3</v>
       </c>
       <c r="J7">
-        <v>0.99573699999999998</v>
+        <v>0.99832500000000002</v>
       </c>
       <c r="K7">
-        <v>1.603E-3</v>
+        <v>4.0900000000000002E-4</v>
       </c>
       <c r="L7">
-        <v>0.99880400000000003</v>
+        <v>0.99948899999999996</v>
       </c>
       <c r="M7">
-        <v>8.1499999999999997E-4</v>
+        <v>1.54E-4</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -933,7 +933,526 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16703012-E066-4FEB-8C35-78B35F85B9FD}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="8" max="8" width="22.5" customWidth="1"/>
+    <col min="9" max="9" width="27.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.5" customWidth="1"/>
+    <col min="11" max="11" width="27" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.97316499999999995</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3.0400000000000002E-3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.99143099999999995</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2.96E-3</v>
+      </c>
+      <c r="F3">
+        <v>0.95747400000000005</v>
+      </c>
+      <c r="G3">
+        <v>4.594E-3</v>
+      </c>
+      <c r="H3">
+        <v>0.97521100000000005</v>
+      </c>
+      <c r="I3" s="4">
+        <v>2.8410000000000002E-3</v>
+      </c>
+      <c r="J3">
+        <v>0.99781399999999998</v>
+      </c>
+      <c r="K3">
+        <v>9.0700000000000004E-4</v>
+      </c>
+      <c r="L3">
+        <v>0.99904800000000005</v>
+      </c>
+      <c r="M3">
+        <v>6.4499999999999996E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.94485699999999995</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5.8339999999999998E-3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.98506300000000002</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5.3309999999999998E-3</v>
+      </c>
+      <c r="F4">
+        <v>0.91237999999999997</v>
+      </c>
+      <c r="G4">
+        <v>8.9820000000000004E-3</v>
+      </c>
+      <c r="H4">
+        <v>0.94853200000000004</v>
+      </c>
+      <c r="I4" s="4">
+        <v>5.1929999999999997E-3</v>
+      </c>
+      <c r="J4">
+        <v>0.99567099999999997</v>
+      </c>
+      <c r="K4">
+        <v>1.9919999999999998E-3</v>
+      </c>
+      <c r="L4">
+        <v>0.99804800000000005</v>
+      </c>
+      <c r="M4">
+        <v>1.302E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.97316499999999995</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3.0400000000000002E-3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.99143099999999995</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2.96E-3</v>
+      </c>
+      <c r="F5">
+        <v>0.95747400000000005</v>
+      </c>
+      <c r="G5">
+        <v>4.594E-3</v>
+      </c>
+      <c r="H5">
+        <v>0.97521100000000005</v>
+      </c>
+      <c r="I5" s="4">
+        <v>2.8410000000000002E-3</v>
+      </c>
+      <c r="J5">
+        <v>0.99781399999999998</v>
+      </c>
+      <c r="K5">
+        <v>9.0700000000000004E-4</v>
+      </c>
+      <c r="L5">
+        <v>0.99904800000000005</v>
+      </c>
+      <c r="M5">
+        <v>6.4499999999999996E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.97316499999999995</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3.0400000000000002E-3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.99143099999999995</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.96E-3</v>
+      </c>
+      <c r="F6">
+        <v>0.95747400000000005</v>
+      </c>
+      <c r="G6">
+        <v>4.594E-3</v>
+      </c>
+      <c r="H6">
+        <v>0.97521100000000005</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2.8410000000000002E-3</v>
+      </c>
+      <c r="J6">
+        <v>0.99781399999999998</v>
+      </c>
+      <c r="K6">
+        <v>9.0700000000000004E-4</v>
+      </c>
+      <c r="L6">
+        <v>0.99904800000000005</v>
+      </c>
+      <c r="M6">
+        <v>6.4499999999999996E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.97316499999999995</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3.0400000000000002E-3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.99143099999999995</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.96E-3</v>
+      </c>
+      <c r="F7">
+        <v>0.95747400000000005</v>
+      </c>
+      <c r="G7">
+        <v>4.594E-3</v>
+      </c>
+      <c r="H7">
+        <v>0.97521100000000005</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2.8410000000000002E-3</v>
+      </c>
+      <c r="J7">
+        <v>0.99781399999999998</v>
+      </c>
+      <c r="K7">
+        <v>9.0700000000000004E-4</v>
+      </c>
+      <c r="L7">
+        <v>0.99904800000000005</v>
+      </c>
+      <c r="M7">
+        <v>6.4499999999999996E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44B21FF-AB14-4997-B4CE-DA44FA76CD12}">
+  <dimension ref="A1:M35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3:M7"/>
     </sheetView>
   </sheetViews>
@@ -992,7 +1511,7 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -1024,40 +1543,40 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>0.98533300000000001</v>
+        <v>0.97015300000000004</v>
       </c>
       <c r="C3" s="3">
-        <v>4.3410000000000002E-3</v>
+        <v>4.0569999999999998E-3</v>
       </c>
       <c r="D3" s="3">
-        <v>0.979715</v>
+        <v>0.985958</v>
       </c>
       <c r="E3" s="3">
-        <v>5.927E-3</v>
+        <v>3.666E-3</v>
       </c>
       <c r="F3">
-        <v>0.83761799999999997</v>
+        <v>0.96161399999999997</v>
       </c>
       <c r="G3">
-        <v>1.3106E-2</v>
+        <v>6.8040000000000002E-3</v>
       </c>
       <c r="H3">
-        <v>0.99043000000000003</v>
+        <v>0.97205799999999998</v>
       </c>
       <c r="I3" s="4">
-        <v>2.8930000000000002E-3</v>
+        <v>3.6749999999999999E-3</v>
       </c>
       <c r="J3">
-        <v>0.99625600000000003</v>
+        <v>0.99640099999999998</v>
       </c>
       <c r="K3">
-        <v>2.5079999999999998E-3</v>
+        <v>1.805E-3</v>
       </c>
       <c r="L3">
-        <v>0.99760800000000005</v>
+        <v>0.99738899999999997</v>
       </c>
       <c r="M3">
-        <v>1.474E-3</v>
+        <v>1.792E-3</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1065,40 +1584,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>0.989259</v>
+        <v>0.93804299999999996</v>
       </c>
       <c r="C4" s="3">
-        <v>3.094E-3</v>
+        <v>6.7600000000000004E-3</v>
       </c>
       <c r="D4" s="3">
-        <v>0.98607900000000004</v>
+        <v>0.97443599999999997</v>
       </c>
       <c r="E4" s="3">
-        <v>4.0969999999999999E-3</v>
+        <v>6.8009999999999998E-3</v>
       </c>
       <c r="F4">
-        <v>0.88017299999999998</v>
+        <v>0.92161999999999999</v>
       </c>
       <c r="G4">
-        <v>8.5609999999999992E-3</v>
+        <v>1.2694E-2</v>
       </c>
       <c r="H4">
-        <v>0.99313899999999999</v>
+        <v>0.94165600000000005</v>
       </c>
       <c r="I4" s="4">
-        <v>2.0869999999999999E-3</v>
+        <v>5.5319999999999996E-3</v>
       </c>
       <c r="J4">
-        <v>0.99726899999999996</v>
+        <v>0.99287700000000001</v>
       </c>
       <c r="K4">
-        <v>1.877E-3</v>
+        <v>3.3649999999999999E-3</v>
       </c>
       <c r="L4">
-        <v>0.99829900000000005</v>
+        <v>0.99478299999999997</v>
       </c>
       <c r="M4">
-        <v>1.0610000000000001E-3</v>
+        <v>3.4789999999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1106,40 +1625,40 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>0.98533300000000001</v>
+        <v>0.97015300000000004</v>
       </c>
       <c r="C5" s="3">
-        <v>4.3410000000000002E-3</v>
+        <v>4.0569999999999998E-3</v>
       </c>
       <c r="D5" s="3">
-        <v>0.979715</v>
+        <v>0.985958</v>
       </c>
       <c r="E5" s="3">
-        <v>5.927E-3</v>
+        <v>3.666E-3</v>
       </c>
       <c r="F5">
-        <v>0.83761799999999997</v>
+        <v>0.96161399999999997</v>
       </c>
       <c r="G5">
-        <v>1.3106E-2</v>
+        <v>6.8040000000000002E-3</v>
       </c>
       <c r="H5">
-        <v>0.99043000000000003</v>
+        <v>0.97205799999999998</v>
       </c>
       <c r="I5" s="4">
-        <v>2.8930000000000002E-3</v>
+        <v>3.6749999999999999E-3</v>
       </c>
       <c r="J5">
-        <v>0.99625600000000003</v>
+        <v>0.99640099999999998</v>
       </c>
       <c r="K5">
-        <v>2.5079999999999998E-3</v>
+        <v>1.805E-3</v>
       </c>
       <c r="L5">
-        <v>0.99760800000000005</v>
+        <v>0.99738899999999997</v>
       </c>
       <c r="M5">
-        <v>1.474E-3</v>
+        <v>1.792E-3</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1147,40 +1666,40 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>0.98533300000000001</v>
+        <v>0.97015300000000004</v>
       </c>
       <c r="C6" s="3">
-        <v>4.3410000000000002E-3</v>
+        <v>4.0569999999999998E-3</v>
       </c>
       <c r="D6" s="3">
-        <v>0.979715</v>
+        <v>0.985958</v>
       </c>
       <c r="E6" s="3">
-        <v>5.927E-3</v>
+        <v>3.666E-3</v>
       </c>
       <c r="F6">
-        <v>0.83761799999999997</v>
+        <v>0.96161399999999997</v>
       </c>
       <c r="G6">
-        <v>1.3106E-2</v>
+        <v>6.8040000000000002E-3</v>
       </c>
       <c r="H6">
-        <v>0.99043000000000003</v>
+        <v>0.97205799999999998</v>
       </c>
       <c r="I6" s="4">
-        <v>2.8930000000000002E-3</v>
+        <v>3.6749999999999999E-3</v>
       </c>
       <c r="J6">
-        <v>0.99625600000000003</v>
+        <v>0.99640099999999998</v>
       </c>
       <c r="K6">
-        <v>2.5079999999999998E-3</v>
+        <v>1.805E-3</v>
       </c>
       <c r="L6">
-        <v>0.99760800000000005</v>
+        <v>0.99738899999999997</v>
       </c>
       <c r="M6">
-        <v>1.474E-3</v>
+        <v>1.792E-3</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1188,40 +1707,40 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>0.98533300000000001</v>
+        <v>0.97015300000000004</v>
       </c>
       <c r="C7" s="3">
-        <v>4.3410000000000002E-3</v>
+        <v>4.0569999999999998E-3</v>
       </c>
       <c r="D7" s="3">
-        <v>0.979715</v>
+        <v>0.985958</v>
       </c>
       <c r="E7" s="3">
-        <v>5.927E-3</v>
+        <v>3.666E-3</v>
       </c>
       <c r="F7">
-        <v>0.83761799999999997</v>
+        <v>0.96161399999999997</v>
       </c>
       <c r="G7">
-        <v>1.3106E-2</v>
+        <v>6.8040000000000002E-3</v>
       </c>
       <c r="H7">
-        <v>0.99043000000000003</v>
+        <v>0.97205799999999998</v>
       </c>
       <c r="I7" s="4">
-        <v>2.8930000000000002E-3</v>
+        <v>3.6749999999999999E-3</v>
       </c>
       <c r="J7">
-        <v>0.99625600000000003</v>
+        <v>0.99640099999999998</v>
       </c>
       <c r="K7">
-        <v>2.5079999999999998E-3</v>
+        <v>1.805E-3</v>
       </c>
       <c r="L7">
-        <v>0.99760800000000005</v>
+        <v>0.99738899999999997</v>
       </c>
       <c r="M7">
-        <v>1.474E-3</v>
+        <v>1.792E-3</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1448,12 +1967,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44B21FF-AB14-4997-B4CE-DA44FA76CD12}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1511,7 +2030,7 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -1523,7 +2042,7 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
@@ -1543,40 +2062,40 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>0.98188200000000003</v>
+        <v>0.96709500000000004</v>
       </c>
       <c r="C3" s="3">
-        <v>6.45E-3</v>
+        <v>5.2859999999999999E-3</v>
       </c>
       <c r="D3" s="3">
-        <v>0.976684</v>
+        <v>0.984182</v>
       </c>
       <c r="E3" s="3">
-        <v>5.437E-3</v>
+        <v>6.7190000000000001E-3</v>
       </c>
       <c r="F3">
-        <v>0.85675500000000004</v>
+        <v>0.96187</v>
       </c>
       <c r="G3">
-        <v>1.4896E-2</v>
+        <v>5.1989999999999996E-3</v>
       </c>
       <c r="H3">
-        <v>0.98708899999999999</v>
+        <v>0.96907299999999996</v>
       </c>
       <c r="I3" s="4">
-        <v>3.784E-3</v>
+        <v>3.2880000000000001E-3</v>
       </c>
       <c r="J3">
-        <v>0.99312900000000004</v>
+        <v>0.99350300000000002</v>
       </c>
       <c r="K3">
-        <v>3.6800000000000001E-3</v>
+        <v>3.4090000000000001E-3</v>
       </c>
       <c r="L3">
-        <v>0.992506</v>
+        <v>0.99322100000000002</v>
       </c>
       <c r="M3">
-        <v>3.947E-3</v>
+        <v>3.9839999999999997E-3</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1584,40 +2103,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>0.98659600000000003</v>
+        <v>0.93111699999999997</v>
       </c>
       <c r="C4" s="3">
-        <v>4.522E-3</v>
+        <v>1.0786E-2</v>
       </c>
       <c r="D4" s="3">
-        <v>0.98248800000000003</v>
+        <v>0.96843400000000002</v>
       </c>
       <c r="E4" s="3">
-        <v>5.5719999999999997E-3</v>
+        <v>1.2518E-2</v>
       </c>
       <c r="F4">
-        <v>0.89317800000000003</v>
+        <v>0.92268700000000003</v>
       </c>
       <c r="G4">
-        <v>7.5310000000000004E-3</v>
+        <v>1.4891E-2</v>
       </c>
       <c r="H4">
-        <v>0.99060300000000001</v>
+        <v>0.93621799999999999</v>
       </c>
       <c r="I4" s="4">
-        <v>2.6080000000000001E-3</v>
+        <v>8.6440000000000006E-3</v>
       </c>
       <c r="J4">
-        <v>0.99467399999999995</v>
+        <v>0.98671399999999998</v>
       </c>
       <c r="K4">
-        <v>2.9520000000000002E-3</v>
+        <v>6.502E-3</v>
       </c>
       <c r="L4">
-        <v>0.99422200000000005</v>
+        <v>0.98614500000000005</v>
       </c>
       <c r="M4">
-        <v>2.993E-3</v>
+        <v>7.5529999999999998E-3</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1625,40 +2144,40 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>0.98188200000000003</v>
+        <v>0.96709500000000004</v>
       </c>
       <c r="C5" s="3">
-        <v>6.45E-3</v>
+        <v>5.2859999999999999E-3</v>
       </c>
       <c r="D5" s="3">
-        <v>0.976684</v>
+        <v>0.984182</v>
       </c>
       <c r="E5" s="3">
-        <v>5.437E-3</v>
+        <v>6.7190000000000001E-3</v>
       </c>
       <c r="F5">
-        <v>0.85675500000000004</v>
+        <v>0.96187</v>
       </c>
       <c r="G5">
-        <v>1.4896E-2</v>
+        <v>5.1989999999999996E-3</v>
       </c>
       <c r="H5">
-        <v>0.98708899999999999</v>
+        <v>0.96907299999999996</v>
       </c>
       <c r="I5" s="4">
-        <v>3.784E-3</v>
+        <v>3.2880000000000001E-3</v>
       </c>
       <c r="J5">
-        <v>0.99312900000000004</v>
+        <v>0.99350300000000002</v>
       </c>
       <c r="K5">
-        <v>3.6800000000000001E-3</v>
+        <v>3.4090000000000001E-3</v>
       </c>
       <c r="L5">
-        <v>0.992506</v>
+        <v>0.99322100000000002</v>
       </c>
       <c r="M5">
-        <v>3.947E-3</v>
+        <v>3.9839999999999997E-3</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1666,40 +2185,40 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>0.98188200000000003</v>
+        <v>0.96709500000000004</v>
       </c>
       <c r="C6" s="3">
-        <v>6.45E-3</v>
+        <v>5.2859999999999999E-3</v>
       </c>
       <c r="D6" s="3">
-        <v>0.976684</v>
+        <v>0.984182</v>
       </c>
       <c r="E6" s="3">
-        <v>5.437E-3</v>
+        <v>6.7190000000000001E-3</v>
       </c>
       <c r="F6">
-        <v>0.85675500000000004</v>
+        <v>0.96187</v>
       </c>
       <c r="G6">
-        <v>1.4896E-2</v>
+        <v>5.1989999999999996E-3</v>
       </c>
       <c r="H6">
-        <v>0.98708899999999999</v>
+        <v>0.96907299999999996</v>
       </c>
       <c r="I6" s="4">
-        <v>3.784E-3</v>
+        <v>3.2880000000000001E-3</v>
       </c>
       <c r="J6">
-        <v>0.99312900000000004</v>
+        <v>0.99350300000000002</v>
       </c>
       <c r="K6">
-        <v>3.6800000000000001E-3</v>
+        <v>3.4090000000000001E-3</v>
       </c>
       <c r="L6">
-        <v>0.992506</v>
+        <v>0.99322100000000002</v>
       </c>
       <c r="M6">
-        <v>3.947E-3</v>
+        <v>3.9839999999999997E-3</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1707,559 +2226,40 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>0.98188200000000003</v>
+        <v>0.96709500000000004</v>
       </c>
       <c r="C7" s="3">
-        <v>6.45E-3</v>
+        <v>5.2859999999999999E-3</v>
       </c>
       <c r="D7" s="3">
-        <v>0.976684</v>
+        <v>0.984182</v>
       </c>
       <c r="E7" s="3">
-        <v>5.437E-3</v>
+        <v>6.7190000000000001E-3</v>
       </c>
       <c r="F7">
-        <v>0.85675500000000004</v>
+        <v>0.96187</v>
       </c>
       <c r="G7">
-        <v>1.4896E-2</v>
+        <v>5.1989999999999996E-3</v>
       </c>
       <c r="H7">
-        <v>0.98708899999999999</v>
+        <v>0.96907299999999996</v>
       </c>
       <c r="I7" s="4">
-        <v>3.784E-3</v>
+        <v>3.2880000000000001E-3</v>
       </c>
       <c r="J7">
-        <v>0.99312900000000004</v>
+        <v>0.99350300000000002</v>
       </c>
       <c r="K7">
-        <v>3.6800000000000001E-3</v>
+        <v>3.4090000000000001E-3</v>
       </c>
       <c r="L7">
-        <v>0.992506</v>
+        <v>0.99322100000000002</v>
       </c>
       <c r="M7">
-        <v>3.947E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M35"/>
-  <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="29.5" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="22.5" customWidth="1"/>
-    <col min="9" max="9" width="27.6640625" customWidth="1"/>
-    <col min="10" max="10" width="21.5" customWidth="1"/>
-    <col min="11" max="11" width="27" customWidth="1"/>
-    <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="13" width="21.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="5"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.97289599999999998</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1.3358999999999999E-2</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.95369800000000005</v>
-      </c>
-      <c r="E3" s="3">
-        <v>2.0077000000000001E-2</v>
-      </c>
-      <c r="F3">
-        <v>0.85112299999999996</v>
-      </c>
-      <c r="G3">
-        <v>2.1642999999999999E-2</v>
-      </c>
-      <c r="H3">
-        <v>0.97998399999999997</v>
-      </c>
-      <c r="I3" s="4">
-        <v>1.0357999999999999E-2</v>
-      </c>
-      <c r="J3">
-        <v>0.98499000000000003</v>
-      </c>
-      <c r="K3">
-        <v>4.0179999999999999E-3</v>
-      </c>
-      <c r="L3">
-        <v>0.98206599999999999</v>
-      </c>
-      <c r="M3">
-        <v>6.8360000000000001E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.97950800000000005</v>
-      </c>
-      <c r="C4" s="3">
-        <v>9.528E-3</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.96701899999999996</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.2864E-2</v>
-      </c>
-      <c r="F4">
-        <v>0.88552200000000003</v>
-      </c>
-      <c r="G4">
-        <v>2.2849999999999999E-2</v>
-      </c>
-      <c r="H4">
-        <v>0.98531299999999999</v>
-      </c>
-      <c r="I4" s="4">
-        <v>6.9899999999999997E-3</v>
-      </c>
-      <c r="J4">
-        <v>0.98333999999999999</v>
-      </c>
-      <c r="K4">
-        <v>1.6899999999999998E-2</v>
-      </c>
-      <c r="L4">
-        <v>0.98627900000000002</v>
-      </c>
-      <c r="M4">
-        <v>5.28E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.97289599999999998</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1.3358999999999999E-2</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.95369800000000005</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2.0077000000000001E-2</v>
-      </c>
-      <c r="F5">
-        <v>0.85112299999999996</v>
-      </c>
-      <c r="G5">
-        <v>2.1642999999999999E-2</v>
-      </c>
-      <c r="H5">
-        <v>0.97998399999999997</v>
-      </c>
-      <c r="I5" s="4">
-        <v>1.0357999999999999E-2</v>
-      </c>
-      <c r="J5">
-        <v>0.98499000000000003</v>
-      </c>
-      <c r="K5">
-        <v>4.0179999999999999E-3</v>
-      </c>
-      <c r="L5">
-        <v>0.98206599999999999</v>
-      </c>
-      <c r="M5">
-        <v>6.8360000000000001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.97289599999999998</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.3358999999999999E-2</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.95369800000000005</v>
-      </c>
-      <c r="E6" s="3">
-        <v>2.0077000000000001E-2</v>
-      </c>
-      <c r="F6">
-        <v>0.85112299999999996</v>
-      </c>
-      <c r="G6">
-        <v>2.1642999999999999E-2</v>
-      </c>
-      <c r="H6">
-        <v>0.97998399999999997</v>
-      </c>
-      <c r="I6" s="4">
-        <v>1.0357999999999999E-2</v>
-      </c>
-      <c r="J6">
-        <v>0.98499000000000003</v>
-      </c>
-      <c r="K6">
-        <v>4.0179999999999999E-3</v>
-      </c>
-      <c r="L6">
-        <v>0.98206599999999999</v>
-      </c>
-      <c r="M6">
-        <v>6.8360000000000001E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.97289599999999998</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.3358999999999999E-2</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.95369800000000005</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2.0077000000000001E-2</v>
-      </c>
-      <c r="F7">
-        <v>0.85112299999999996</v>
-      </c>
-      <c r="G7">
-        <v>2.1642999999999999E-2</v>
-      </c>
-      <c r="H7">
-        <v>0.97998399999999997</v>
-      </c>
-      <c r="I7" s="4">
-        <v>1.0357999999999999E-2</v>
-      </c>
-      <c r="J7">
-        <v>0.98499000000000003</v>
-      </c>
-      <c r="K7">
-        <v>4.0179999999999999E-3</v>
-      </c>
-      <c r="L7">
-        <v>0.98206599999999999</v>
-      </c>
-      <c r="M7">
-        <v>6.8360000000000001E-3</v>
+        <v>3.9839999999999997E-3</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>